<commit_message>
orden + login shinymanager
</commit_message>
<xml_diff>
--- a/data/users.xlsx
+++ b/data/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\visor-smartdata\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4350E2-95DE-498C-AB32-BD26D533AFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDFDA98-7848-4266-AED3-2FB158835414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8520" yWindow="4275" windowWidth="28800" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8640" yWindow="2610" windowWidth="28800" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>user</t>
   </si>
@@ -33,30 +33,12 @@
     <t>password</t>
   </si>
   <si>
-    <t>permission</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>Administrador</t>
-  </si>
-  <si>
-    <t>standard</t>
-  </si>
-  <si>
     <t>usuario</t>
   </si>
   <si>
-    <t>Juan Perez</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
     <t>&amp;XCZ9c^e82TirE</t>
   </si>
   <si>
@@ -67,6 +49,12 @@
   </si>
   <si>
     <t>clave</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
@@ -131,13 +119,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D994ECC9-E785-4720-AD1D-EDBE8EC9A7CD}" name="Tabla1" displayName="Tabla1" ref="A1:D4" totalsRowShown="0">
-  <autoFilter ref="A1:D4" xr:uid="{D994ECC9-E785-4720-AD1D-EDBE8EC9A7CD}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D994ECC9-E785-4720-AD1D-EDBE8EC9A7CD}" name="Tabla1" displayName="Tabla1" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4" xr:uid="{D994ECC9-E785-4720-AD1D-EDBE8EC9A7CD}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{814E2861-7D55-40E6-A1E2-557BAD329761}" name="user"/>
     <tableColumn id="2" xr3:uid="{2703FDD1-683A-4411-8171-E0E053BABED8}" name="password"/>
-    <tableColumn id="3" xr3:uid="{8B5153DF-81EE-4A55-A606-6E014876073D}" name="permission"/>
-    <tableColumn id="4" xr3:uid="{99ED9C21-5E82-4842-9B76-2183107BB0CB}" name="name"/>
+    <tableColumn id="3" xr3:uid="{FA827503-D59B-41C3-BCBD-D3EFA499166D}" name="admin"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -406,21 +393,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,54 +415,42 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I8" s="1"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>